<commit_message>
Utworzenie arkusza dla najczesciej wypozyczanych egzemplarzy
</commit_message>
<xml_diff>
--- a/ProjektBiblioteka/bin/Debug/mostpopularbook.xlsx
+++ b/ProjektBiblioteka/bin/Debug/mostpopularbook.xlsx
@@ -63,7 +63,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -79,7 +79,90 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>10</v>
+        <v>8</v>
+      </c>
+      <c r="B2" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0">
+        <v>1</v>
+      </c>
+      <c r="B3" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0">
+        <v>2</v>
+      </c>
+      <c r="B4" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0">
+        <v>3</v>
+      </c>
+      <c r="B5" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0">
+        <v>4</v>
+      </c>
+      <c r="B6" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0">
+        <v>5</v>
+      </c>
+      <c r="B7" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0">
+        <v>6</v>
+      </c>
+      <c r="B8" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0">
+        <v>7</v>
+      </c>
+      <c r="B9" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0">
+        <v>12</v>
+      </c>
+      <c r="B10" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0">
+        <v>13</v>
+      </c>
+      <c r="B11" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0">
+        <v>32</v>
+      </c>
+      <c r="B12" s="0">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dodanie diagramu do excela (do poprawy dodanie miesięcy)
</commit_message>
<xml_diff>
--- a/ProjektBiblioteka/bin/Debug/mostpopularbook.xlsx
+++ b/ProjektBiblioteka/bin/Debug/mostpopularbook.xlsx
@@ -104,6 +104,199 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1080" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:effectLst/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr/>
+              <a:t>Best Book chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Filary ziemi</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'BestBook (ALL)'!$A$1:$B$1</c:f>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'BestBook (ALL)'!$A$2:$B$2</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Uciekinier</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'BestBook (ALL)'!$A$1:$B$1</c:f>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'BestBook (ALL)'!$A$4:$B$4</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:smooth val="0"/>
+        <c:axId val="1"/>
+        <c:axId val="2"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr kern="1200" sz="900"/>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr kern="1200" sz="900"/>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr anchorCtr="1" anchor="ctr" wrap="square" vert="horz" vertOverflow="ellipsis" spcFirstLastPara="1" rot="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <graphicFrame xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="lineChart"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
   <dimension ref="A1:B7"/>
@@ -174,6 +367,7 @@
     </row>
   </sheetData>
   <headerFooter/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Poprawki - data, doplaty
</commit_message>
<xml_diff>
--- a/ProjektBiblioteka/bin/Debug/mostpopularbook.xlsx
+++ b/ProjektBiblioteka/bin/Debug/mostpopularbook.xlsx
@@ -5,26 +5,26 @@
     <workbookView/>
   </bookViews>
   <sheets>
-    <sheet name="BestBook (ALL)" sheetId="1" r:id="rId1"/>
-    <sheet name="January" sheetId="2" r:id="rId2"/>
-    <sheet name="February" sheetId="3" r:id="rId3"/>
-    <sheet name="March" sheetId="4" r:id="rId4"/>
-    <sheet name="April" sheetId="5" r:id="rId5"/>
-    <sheet name="May" sheetId="6" r:id="rId6"/>
-    <sheet name="June" sheetId="7" r:id="rId7"/>
-    <sheet name="July" sheetId="8" r:id="rId8"/>
-    <sheet name="August" sheetId="9" r:id="rId9"/>
-    <sheet name="September" sheetId="10" r:id="rId10"/>
-    <sheet name="October" sheetId="11" r:id="rId11"/>
-    <sheet name="November" sheetId="12" r:id="rId12"/>
-    <sheet name="December" sheetId="13" r:id="rId13"/>
+    <sheet name="styczeń" sheetId="1" r:id="rId1"/>
+    <sheet name="luty" sheetId="2" r:id="rId2"/>
+    <sheet name="marzec" sheetId="3" r:id="rId3"/>
+    <sheet name="kwiecień" sheetId="4" r:id="rId4"/>
+    <sheet name="maj" sheetId="5" r:id="rId5"/>
+    <sheet name="czerwiec" sheetId="6" r:id="rId6"/>
+    <sheet name="lipiec" sheetId="7" r:id="rId7"/>
+    <sheet name="sierpień" sheetId="8" r:id="rId8"/>
+    <sheet name="wrzesień" sheetId="9" r:id="rId9"/>
+    <sheet name="październik" sheetId="10" r:id="rId10"/>
+    <sheet name="listopad" sheetId="11" r:id="rId11"/>
+    <sheet name="grudzień" sheetId="12" r:id="rId12"/>
+    <sheet name="BestBook (ALL)" sheetId="13" r:id="rId13"/>
   </sheets>
   <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Id</t>
   </si>
@@ -35,13 +35,19 @@
     <t>Date (month-year)</t>
   </si>
   <si>
-    <t>C# 7.0 Kompletny przewodnik dla praktyków</t>
+    <t>Mistyfikacja</t>
+  </si>
+  <si>
+    <t>Szkarłatna wdowa</t>
+  </si>
+  <si>
+    <t>Uciekinier</t>
   </si>
   <si>
     <t>Filary ziemi</t>
   </si>
   <si>
-    <t>Uciekinier</t>
+    <t>C# 7.0 Kompletny przewodnik dla praktyków</t>
   </si>
   <si>
     <t>Władca Barcelony</t>
@@ -49,16 +55,13 @@
   <si>
     <t>Norwegian Wood</t>
   </si>
-  <si>
-    <t>Szkarłatna wdowa</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="mm-yyyy"/>
+    <numFmt numFmtId="164" formatCode="mmm-yyyy"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -249,6 +252,34 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>
+              </c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'BestBook (ALL)'!$A$1:$B$1</c:f>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'BestBook (ALL)'!$A$10:$B$10</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
         <c:smooth val="0"/>
         <c:axId val="1"/>
         <c:axId val="2"/>
@@ -324,7 +355,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing13.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -361,15 +392,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
-  <dimension ref="A1:C7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" hidden="1" width="20" customWidth="1"/>
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="20" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -388,7 +419,10 @@
         <v>3</v>
       </c>
       <c r="B2" s="0">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="C2" s="2">
+        <v>44202</v>
       </c>
     </row>
     <row r="3">
@@ -396,7 +430,10 @@
         <v>4</v>
       </c>
       <c r="B3" s="0">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="C3" s="2">
+        <v>44202</v>
       </c>
     </row>
     <row r="4">
@@ -404,7 +441,10 @@
         <v>5</v>
       </c>
       <c r="B4" s="0">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="C4" s="2">
+        <v>44199</v>
       </c>
     </row>
     <row r="5">
@@ -412,34 +452,49 @@
         <v>6</v>
       </c>
       <c r="B5" s="0">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="0">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="0">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <headerFooter/>
-  <drawing r:id="rId1"/>
+        <v>1</v>
+      </c>
+      <c r="C5" s="2">
+        <v>43850</v>
+      </c>
+    </row>
+  </sheetData>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="20" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -463,45 +518,13 @@
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B2" s="0">
         <v>1</v>
       </c>
       <c r="C2" s="2">
-        <v>44096</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="C3" s="2"/>
-    </row>
-  </sheetData>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="20" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>44160</v>
       </c>
     </row>
   </sheetData>
@@ -511,7 +534,7 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -535,50 +558,7 @@
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="0">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2">
-        <v>44160</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="C3" s="2"/>
-    </row>
-  </sheetData>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
-  <dimension ref="A1:C6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="20" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="0" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B2" s="0">
         <v>3</v>
@@ -589,7 +569,7 @@
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B3" s="0">
         <v>2</v>
@@ -611,7 +591,7 @@
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B5" s="0">
         <v>1</v>
@@ -620,25 +600,22 @@
         <v>44195</v>
       </c>
     </row>
-    <row r="6">
-      <c r="C6" s="2"/>
-    </row>
-  </sheetData>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="20" customWidth="1"/>
+  </sheetData>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" hidden="1" width="20" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -654,24 +631,88 @@
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B2" s="0">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2">
-        <v>44199</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="0">
-        <v>1</v>
-      </c>
-      <c r="C3" s="2">
-        <v>43850</v>
+      <c r="B7" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="0">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <headerFooter/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="20" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -768,36 +809,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="20" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -821,7 +833,7 @@
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B2" s="0">
         <v>1</v>
@@ -830,8 +842,34 @@
         <v>43990</v>
       </c>
     </row>
-    <row r="3">
-      <c r="C3" s="2"/>
+  </sheetData>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="20" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <headerFooter/>
@@ -840,36 +878,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="20" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -893,7 +902,7 @@
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B2" s="0">
         <v>1</v>
@@ -902,8 +911,45 @@
         <v>44061</v>
       </c>
     </row>
-    <row r="3">
-      <c r="C3" s="2"/>
+  </sheetData>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="20" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="0">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2">
+        <v>44096</v>
+      </c>
     </row>
   </sheetData>
   <headerFooter/>

</xml_diff>